<commit_message>
apply random forest model
</commit_message>
<xml_diff>
--- a/irm_final_evaluation/datasets/codebook.xlsx
+++ b/irm_final_evaluation/datasets/codebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\myagh\fc-performeter\irm_final_evaluation\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9FCF55-AF52-4358-A1AD-94EB80EEB9FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7468C5FE-7B78-4A72-9F8B-427AB9DA0696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3A815EF1-E797-4900-B675-83DD241DD288}"/>
   </bookViews>
@@ -966,7 +966,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -976,6 +976,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1020,7 +1026,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1041,6 +1047,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1648,8 +1660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{148F1E3C-688D-4908-8A07-024E3424870C}">
   <dimension ref="A1:T123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2142,16 +2154,16 @@
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="3">
-        <v>1</v>
-      </c>
-      <c r="D19" s="3" t="s">
+      <c r="C19" s="9">
+        <v>1</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="9" t="s">
         <v>85</v>
       </c>
       <c r="G19" s="3" t="s">
@@ -2703,16 +2715,16 @@
       <c r="A34" s="1">
         <v>32</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C34" s="3">
-        <v>1</v>
-      </c>
-      <c r="D34" s="3" t="s">
+      <c r="C34" s="9">
+        <v>1</v>
+      </c>
+      <c r="D34" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="9" t="s">
         <v>126</v>
       </c>
       <c r="G34" s="3" t="s">

</xml_diff>